<commit_message>
Initial commit - GroceryBot project
</commit_message>
<xml_diff>
--- a/GroceryRequests.xlsx
+++ b/GroceryRequests.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,159 +438,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2025-09-25 18:30:49</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Jacob Sandau</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>apples</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2025-09-25 18:32:59</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Jacob Sandau</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>apples</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2025-09-25 18:33:06</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Jacob Sandau</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>bananas</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2025-09-25 18:33:12</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Jacob Sandau</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>bread</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2025-09-25 18:34:56</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Jacob Sandau</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>apples</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2025-10-13 19:52:08</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Jacob Sandau</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>apples</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2025-10-13 19:52:25</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Jacob Sandau</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>cereal</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2025-10-13 19:52:55</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Jacob Sandau</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>bananas</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2025-10-13 19:53:50</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Jacob Sandau</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>seasoned salt</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>